<commit_message>
Home Page features test script completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E52DA3-F61B-4623-8A3E-458E204D23AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95E1A1-C07A-4BB4-8C8A-AE2CD8638098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1118" yWindow="1125" windowWidth="16140" windowHeight="9285" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
     <sheet name="TestScripts" sheetId="3" r:id="rId3"/>
     <sheet name="LoginTestData" sheetId="4" r:id="rId4"/>
-    <sheet name="InvalidLoginScenarios" sheetId="8" r:id="rId5"/>
-    <sheet name="SearchJavaCourse" sheetId="5" r:id="rId6"/>
-    <sheet name="SearchPageFilters" sheetId="6" r:id="rId7"/>
-    <sheet name="CoursePageDetails" sheetId="7" r:id="rId8"/>
-    <sheet name="CheckExternalLinks" sheetId="9" r:id="rId9"/>
+    <sheet name="NegativeLoginScenarios" sheetId="8" r:id="rId5"/>
+    <sheet name="CoursePageDetails" sheetId="7" r:id="rId6"/>
+    <sheet name="HomePageFeatures" sheetId="10" r:id="rId7"/>
+    <sheet name="SearchPageFeatures" sheetId="5" r:id="rId8"/>
+    <sheet name="JavaSearchFunctionality" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -119,79 +119,264 @@
     <t>LoginType</t>
   </si>
   <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>ExpSearchText</t>
+  </si>
+  <si>
+    <t>What do you want to learn?</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>User4</t>
+  </si>
+  <si>
+    <t>User5</t>
+  </si>
+  <si>
+    <t>TC_0002_1</t>
+  </si>
+  <si>
+    <t>TC_0002_2</t>
+  </si>
+  <si>
+    <t>TC_0002_3</t>
+  </si>
+  <si>
+    <t>TC_0002_4</t>
+  </si>
+  <si>
+    <t>TC_0002_5</t>
+  </si>
+  <si>
+    <t>notadmin</t>
+  </si>
+  <si>
+    <t>notpassword</t>
+  </si>
+  <si>
+    <t>password125</t>
+  </si>
+  <si>
+    <t>Invalid user name or password</t>
+  </si>
+  <si>
+    <t>ExpErrorMessage</t>
+  </si>
+  <si>
+    <t>C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\LoginPage.html</t>
+  </si>
+  <si>
+    <r>
+      <t>verify</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>LoginPageNegative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Scenarios</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>verify</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>HomePage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Features</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>verify</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CoursePage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Features</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>verify</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SearchPage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Features</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>verify</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>JavaSearch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Functionality</t>
+    </r>
+  </si>
+  <si>
+    <t>NegativeLoginScenarios</t>
+  </si>
+  <si>
+    <t>HomePageFeatures</t>
+  </si>
+  <si>
+    <t>CoursePageDetails</t>
+  </si>
+  <si>
+    <t>SearchPageFeatures</t>
+  </si>
+  <si>
+    <t>JavaSearchFunctionality</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>CoursePage</t>
+  </si>
+  <si>
+    <t>SearchPage</t>
+  </si>
+  <si>
+    <t>JavaSearch</t>
+  </si>
+  <si>
+    <t>TC_0003_1</t>
+  </si>
+  <si>
+    <t>TC_0003_2</t>
+  </si>
+  <si>
+    <t>TC_0004_1</t>
+  </si>
+  <si>
+    <t>TC_0004_2</t>
+  </si>
+  <si>
+    <t>TC_0005_1</t>
+  </si>
+  <si>
+    <t>TC_0005_2</t>
+  </si>
+  <si>
+    <t>TC_0006_1</t>
+  </si>
+  <si>
+    <t>TC_0006_2</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>password123</t>
-  </si>
-  <si>
-    <t>ExpSearchText</t>
-  </si>
-  <si>
-    <t>What do you want to learn?</t>
-  </si>
-  <si>
-    <t>User3</t>
-  </si>
-  <si>
-    <t>User4</t>
-  </si>
-  <si>
-    <t>User5</t>
-  </si>
-  <si>
-    <t>TC_0002_1</t>
-  </si>
-  <si>
-    <t>TC_0002_2</t>
-  </si>
-  <si>
-    <t>TC_0002_3</t>
-  </si>
-  <si>
-    <t>TC_0002_4</t>
-  </si>
-  <si>
-    <t>TC_0002_5</t>
-  </si>
-  <si>
-    <t>notadmin</t>
-  </si>
-  <si>
-    <t>notpassword</t>
-  </si>
-  <si>
-    <t>password125</t>
-  </si>
-  <si>
-    <t>Invalid user name or password</t>
-  </si>
-  <si>
-    <t>ExpErrorMessage</t>
-  </si>
-  <si>
-    <t>C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\LoginPage.html</t>
-  </si>
-  <si>
     <t>100.0 %</t>
   </si>
   <si>
+    <t>ExpHomePageHeader</t>
+  </si>
+  <si>
+    <t>ExpHomePageDesc</t>
+  </si>
+  <si>
+    <t>The technology
+learning platform</t>
+  </si>
+  <si>
     <t>FAIL</t>
   </si>
   <si>
     <t>0.0 %</t>
+  </si>
+  <si>
+    <t>Keep up with technology with expert-led courses, assessments and tools that help you build the skills you need, when you need them.
+For organizations, get unprecedented insight into skills strengths and weaknesses and align learning to what matters.</t>
   </si>
 </sst>
 </file>
@@ -201,7 +386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +471,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,11 +534,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
@@ -506,7 +694,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -515,7 +703,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
@@ -541,26 +728,45 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -854,20 +1060,20 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="47.86328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="43.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
@@ -886,13 +1092,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.19921875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
   </cols>
   <sheetData>
@@ -905,20 +1111,20 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>45</v>
+      <c r="B2" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -938,7 +1144,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -946,109 +1152,147 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="8.1328125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="33.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s" s="39">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s" s="41">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="18" t="s">
+      <c r="C6" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
+      <c r="B7" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1059,6 +1303,11 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" location="LoginTestData!A1" display="LoginTestData" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" location="NegativeLoginScenarios!A1" display="NegativeLoginScenarios" xr:uid="{29E5C240-744F-4C7F-B661-4F37CAFD8CD6}"/>
+    <hyperlink ref="C4" location="HomePageFeatures!A1" display="HomePageFeatures" xr:uid="{6B9E9C52-52FF-43EE-A6F3-296A353C5448}"/>
+    <hyperlink ref="C5" location="CoursePageDetails!A1" display="CoursePageDetails" xr:uid="{09E898F7-1ECF-414F-9E7F-B4AFA353D3E3}"/>
+    <hyperlink ref="C6" location="SearchPageFeatures!A1" display="SearchPageFeatures" xr:uid="{D070B42A-2337-4430-A94E-383B16D6F5C3}"/>
+    <hyperlink ref="C7" location="JavaSearchFunctionality!A1" display="JavaSearchFunctionality" xr:uid="{F7351B57-B1F4-48FB-A3D3-9758E5479FFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1070,87 +1319,87 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.86328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.86328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="12.265625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="24.46484375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.59765625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="7.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="G2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>47</v>
+      <c r="F3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1421,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1187,133 +1436,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="25" t="s">
+      <c r="F3" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>24</v>
+      <c r="G6" s="23" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1328,11 +1577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1344,63 +1593,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="E2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>24</v>
+      <c r="D3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{2EB08E7A-9DE2-4D6F-A588-CBA4DB251774}">
-      <formula1>"TC_0001_1,Not To Run"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{97D640AA-990C-4B02-81DF-22AF16A7382C}">
-      <formula1>"TC_0001_2,Not To Run"</formula1>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{8DD5F003-84F9-4453-B61D-C6EE61EACE70}">
+      <formula1>"TC_0003_1,Not To Run"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1408,11 +1655,101 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3356B94C-5B4C-4FFF-9F00-EBBCCEB4F868}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.06640625"/>
+    <col min="5" max="5" customWidth="true" width="59.59765625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
+      <c r="A3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{CE3AAC6A-F7EC-495F-A000-D9D096D0025F}">
+      <formula1>"TC_0004_1,Not To Run"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1424,75 +1761,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="E2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>24</v>
+      <c r="D3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{96725BED-2D94-441F-AEEB-887B2A7B7B74}">
-      <formula1>"TC_0001_2,Not To Run"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{7EE091FA-9632-4F03-8BD6-6DF4BEE70883}">
-      <formula1>"TC_0001_1,Not To Run"</formula1>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{2EB08E7A-9DE2-4D6F-A588-CBA4DB251774}">
+      <formula1>"TC_0005_1,Not To Run"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1504,163 +1839,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="24" t="s">
+      <c r="E2" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>24</v>
+      <c r="D3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{8DD5F003-84F9-4453-B61D-C6EE61EACE70}">
-      <formula1>"TC_0001_1,Not To Run"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{ECC7616D-F15F-4B7F-B209-00B7C6B18F91}">
-      <formula1>"TC_0001_2,Not To Run"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39452479-CCF1-438A-A9AC-213FA6836521}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.265625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.46484375"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{EBA13561-D602-4EFA-AA27-A87C1CD1280E}">
-      <formula1>"TC_0001_2,Not To Run"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C8C53CA6-9714-4027-80EC-E9B460E1ED57}">
-      <formula1>"TC_0001_1,Not To Run"</formula1>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{7EE091FA-9632-4F03-8BD6-6DF4BEE70883}">
+      <formula1>"TC_0006_1,Not To Run"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Negative login scenarios completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD95E1A1-C07A-4BB4-8C8A-AE2CD8638098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE2E12D-22E8-4A2E-AEF2-4490A2BF3553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1118" yWindow="1125" windowWidth="16140" windowHeight="9285" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -369,14 +369,14 @@
 learning platform</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>0.0 %</t>
-  </si>
-  <si>
     <t>Keep up with technology with expert-led courses, assessments and tools that help you build the skills you need, when you need them.
 For organizations, get unprecedented insight into skills strengths and weaknesses and align learning to what matters.</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>0.0 %</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +534,11 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
@@ -694,7 +699,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -763,7 +768,31 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1144,7 +1173,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1210,9 +1239,11 @@
       <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
+      <c r="E3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s" s="63">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1231,7 +1262,7 @@
       <c r="E4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s" s="39">
+      <c r="F4" s="28" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1418,151 +1449,132 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E7E38D-2134-4D7B-AFCC-79142EC6D7FA}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.265625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="27.33203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.06640625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.265625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.33203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="E1" s="7" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>39</v>
       </c>
+      <c r="D2" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="E2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F2" s="58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>26</v>
       </c>
+      <c r="D3" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="E3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F4" s="60" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F5" s="61" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E6" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>22</v>
+      <c r="F6" s="62" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3356B94C-5B4C-4FFF-9F00-EBBCCEB4F868}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1706,9 +1718,9 @@
         <v>71</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1726,9 +1738,9 @@
         <v>71</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed all test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE2E12D-22E8-4A2E-AEF2-4490A2BF3553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5E3076-5631-4B19-A49B-A996D1601A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -111,9 +111,6 @@
       </rPr>
       <t>LoginFunctionality</t>
     </r>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>LoginType</t>
@@ -332,25 +329,13 @@
     <t>TC_0003_1</t>
   </si>
   <si>
-    <t>TC_0003_2</t>
-  </si>
-  <si>
     <t>TC_0004_1</t>
   </si>
   <si>
-    <t>TC_0004_2</t>
-  </si>
-  <si>
     <t>TC_0005_1</t>
   </si>
   <si>
-    <t>TC_0005_2</t>
-  </si>
-  <si>
     <t>TC_0006_1</t>
-  </si>
-  <si>
-    <t>TC_0006_2</t>
   </si>
   <si>
     <t>PASS</t>
@@ -371,6 +356,39 @@
   <si>
     <t>Keep up with technology with expert-led courses, assessments and tools that help you build the skills you need, when you need them.
 For organizations, get unprecedented insight into skills strengths and weaknesses and align learning to what matters.</t>
+  </si>
+  <si>
+    <t>CourseName</t>
+  </si>
+  <si>
+    <t>Java Fundamentals: The Java Language</t>
+  </si>
+  <si>
+    <t>ExpCourseOverviewText</t>
+  </si>
+  <si>
+    <t>ExpFreeTrailText</t>
+  </si>
+  <si>
+    <t>ExpCourseHeaderText</t>
+  </si>
+  <si>
+    <t>ExpCourseDescriptionText</t>
+  </si>
+  <si>
+    <t>This course provides thorough coverage of the core Java platform, giving you the skills needed to begin developing in the Java Runtime Environment (JRE) and serving as a solid foundation for all Java-based development environments.</t>
+  </si>
+  <si>
+    <t>Start a FREE 10-day trial</t>
+  </si>
+  <si>
+    <t>Play course overview</t>
+  </si>
+  <si>
+    <t>Not To Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java </t>
   </si>
   <si>
     <t>FAIL</t>
@@ -544,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -685,6 +703,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -699,7 +728,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,7 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,6 +796,38 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
@@ -778,22 +838,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -1102,7 +1148,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1140,11 +1186,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1220,10 +1266,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1231,19 +1277,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s" s="63">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1251,19 +1297,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>54</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1271,19 +1317,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1291,39 +1337,39 @@
         <v>10</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F6" t="s" s="62">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>49</v>
+      <c r="B7" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="F7" t="s" s="66">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1372,7 +1418,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>13</v>
@@ -1381,7 +1427,7 @@
         <v>15</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>9</v>
@@ -1395,19 +1441,19 @@
         <v>14</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1418,19 +1464,19 @@
         <v>20</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E7E38D-2134-4D7B-AFCC-79142EC6D7FA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1479,7 +1525,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>9</v>
@@ -1490,19 +1536,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1510,71 +1556,71 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="62" t="s">
-        <v>67</v>
+      <c r="F6" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1590,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1601,10 +1647,14 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.46484375"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
+    <col min="6" max="6" customWidth="true" width="69.46484375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.59765625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -1612,47 +1662,83 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.45">
+      <c r="A3" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>67</v>
+      <c r="D3" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1757,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1685,63 +1771,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A2" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="34" t="s">
+      <c r="D2" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
+      <c r="A3" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="D3" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A3" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="33" t="s">
+      <c r="F3" s="27" t="s">
         <v>62</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1760,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1769,7 +1855,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.46484375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -1780,10 +1866,10 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>9</v>
@@ -1794,16 +1880,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>67</v>
+        <v>78</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -1811,16 +1897,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>67</v>
+        <v>78</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1836,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1847,10 +1933,12 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.46484375"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
+    <col min="6" max="6" customWidth="true" style="37" width="69.53125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -1858,47 +1946,65 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>67</v>
+      <c r="D3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logger and encryption/decryption facility to project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5E3076-5631-4B19-A49B-A996D1601A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0D4C6-7F9F-4EF5-8CA4-912C05F4D138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="80">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>User2</t>
-  </si>
-  <si>
-    <t>TC_0001_2</t>
   </si>
   <si>
     <r>
@@ -391,10 +388,10 @@
     <t xml:space="preserve">Java </t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>0.0 %</t>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>TC_0001_2</t>
   </si>
 </sst>
 </file>
@@ -498,7 +495,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,16 +548,6 @@
         <fgColor indexed="50"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -728,7 +715,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,28 +805,27 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
@@ -1135,7 +1121,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1149,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1176,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1257,7 +1243,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -1266,10 +1252,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="27" t="s">
         <v>62</v>
+      </c>
+      <c r="F2" t="s" s="51">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1277,19 +1263,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="27" t="s">
         <v>62</v>
+      </c>
+      <c r="F3" t="s" s="57">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1297,19 +1283,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="27" t="s">
         <v>62</v>
+      </c>
+      <c r="F4" t="s" s="61">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1317,19 +1303,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="27" t="s">
         <v>62</v>
+      </c>
+      <c r="F5" t="s" s="59">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1337,19 +1323,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" t="s" s="62">
         <v>62</v>
+      </c>
+      <c r="F6" t="s" s="63">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1357,19 +1343,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s" s="66">
         <v>62</v>
+      </c>
+      <c r="F7" t="s" s="65">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1418,7 +1404,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>13</v>
@@ -1427,7 +1413,7 @@
         <v>15</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>9</v>
@@ -1441,19 +1427,19 @@
         <v>14</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1461,31 +1447,29 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0300-000000000000}">
+  <phoneticPr fontId="12" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TC_0001_1,Not To Run"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0300-000001000000}">
-      <formula1>"TC_0001_2,Not To Run"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1525,7 +1509,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>9</v>
@@ -1536,19 +1520,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1556,71 +1540,71 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>62</v>
+      <c r="F6" s="56" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1662,22 +1646,22 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>9</v>
@@ -1688,28 +1672,28 @@
         <v>18</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="H2" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>62</v>
+      <c r="I2" s="58" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.45">
@@ -1717,28 +1701,28 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="H3" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="39" t="s">
-        <v>76</v>
-      </c>
       <c r="I3" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1778,13 +1762,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>65</v>
       </c>
       <c r="F1" s="31" t="s">
         <v>9</v>
@@ -1795,19 +1779,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>62</v>
+      <c r="F2" s="60" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
@@ -1815,19 +1799,19 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>67</v>
-      </c>
       <c r="F3" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1846,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1866,10 +1850,10 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>9</v>
@@ -1880,16 +1864,16 @@
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -1897,16 +1881,16 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="E3" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1946,16 +1930,16 @@
         <v>12</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>72</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>73</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>9</v>
@@ -1966,22 +1950,22 @@
         <v>18</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="64" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="65" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
@@ -1989,22 +1973,22 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retry mechanism added for classes and suite
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D0D4C6-7F9F-4EF5-8CA4-912C05F4D138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324FC588-1A28-4AC1-AD84-249B849C29B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="85">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -382,9 +382,6 @@
     <t>Play course overview</t>
   </si>
   <si>
-    <t>Not To Run</t>
-  </si>
-  <si>
     <t xml:space="preserve">Java </t>
   </si>
   <si>
@@ -392,6 +389,24 @@
   </si>
   <si>
     <t>TC_0001_2</t>
+  </si>
+  <si>
+    <t>TC_0005_2</t>
+  </si>
+  <si>
+    <t>TC_0004_2</t>
+  </si>
+  <si>
+    <t>TC_0003_2</t>
+  </si>
+  <si>
+    <t>TC_0006_2</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>0.0 %</t>
   </si>
 </sst>
 </file>
@@ -495,7 +510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +563,16 @@
         <fgColor indexed="50"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -715,7 +740,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,6 +835,96 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1135,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1252,10 +1367,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s" s="51">
-        <v>61</v>
+        <v>84</v>
+      </c>
+      <c r="F2" t="s" s="137">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1274,7 +1389,7 @@
       <c r="E3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="s" s="57">
+      <c r="F3" t="s" s="143">
         <v>61</v>
       </c>
     </row>
@@ -1294,7 +1409,7 @@
       <c r="E4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s" s="61">
+      <c r="F4" t="s" s="149">
         <v>61</v>
       </c>
     </row>
@@ -1314,7 +1429,7 @@
       <c r="E5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F5" t="s" s="59">
+      <c r="F5" t="s" s="146">
         <v>61</v>
       </c>
     </row>
@@ -1334,7 +1449,7 @@
       <c r="E6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F6" t="s" s="63">
+      <c r="F6" t="s" s="152">
         <v>61</v>
       </c>
     </row>
@@ -1354,7 +1469,7 @@
       <c r="E7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s" s="65">
+      <c r="F7" t="s" s="155">
         <v>61</v>
       </c>
     </row>
@@ -1381,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1438,8 +1553,8 @@
       <c r="F2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="49" t="s">
-        <v>61</v>
+      <c r="G2" s="135" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1447,7 +1562,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>23</v>
@@ -1461,8 +1576,8 @@
       <c r="F3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="50" t="s">
-        <v>61</v>
+      <c r="G3" s="136" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1531,7 +1646,7 @@
       <c r="E2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="138" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1551,7 +1666,7 @@
       <c r="E3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="139" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1567,7 +1682,7 @@
       <c r="E4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="140" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1585,7 +1700,7 @@
       <c r="E5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="141" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1603,7 +1718,7 @@
       <c r="E6" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="142" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1623,7 +1738,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1692,7 +1807,7 @@
       <c r="H2" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="58" t="s">
+      <c r="I2" s="144" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1701,7 +1816,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>23</v>
@@ -1721,7 +1836,7 @@
       <c r="H3" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="145" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1741,7 +1856,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1790,7 +1905,7 @@
       <c r="E2" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="147" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1799,7 +1914,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>23</v>
@@ -1810,7 +1925,7 @@
       <c r="E3" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="148" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1831,7 +1946,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1870,9 +1985,9 @@
         <v>22</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="150" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1881,15 +1996,15 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="151" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1908,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1964,7 +2079,7 @@
       <c r="F2" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="153" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1973,7 +2088,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>23</v>
@@ -1987,7 +2102,7 @@
       <c r="F3" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="154" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated project flow and credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324FC588-1A28-4AC1-AD84-249B849C29B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D670B551-72CD-4037-9CA8-05D33E6C6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="87">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -122,9 +122,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
     <t>password123</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
   </si>
   <si>
     <t>ExpErrorMessage</t>
-  </si>
-  <si>
-    <t>C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\LoginPage.html</t>
   </si>
   <si>
     <r>
@@ -406,7 +400,19 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>0.0 %</t>
+    <t>https://nirajt03.github.io/sample-website/</t>
+  </si>
+  <si>
+    <t>test.admin</t>
+  </si>
+  <si>
+    <t>test.user</t>
+  </si>
+  <si>
+    <t>pragyan@123</t>
+  </si>
+  <si>
+    <t>33.33 %</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,8 +515,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,11 +578,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
       </patternFill>
@@ -740,7 +749,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -751,7 +760,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -824,107 +832,22 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1249,8 +1172,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>77</v>
+      <c r="B1" s="22" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1269,13 +1192,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="8.19921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -1287,11 +1210,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
+      <c r="B2" s="42" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1305,7 +1228,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{10B06994-FAE1-44A6-AECD-A0F9FA11DEA7}">
-      <formula1>"C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\LoginPage.html,C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\HomePage.html,https://www.google.com"</formula1>
+      <formula1>"https://nirajt03.github.io/sample-website/,https://www.google.com,C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\main\resources\WebPages\LoginPage.html"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1334,143 +1257,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s" s="137">
-        <v>83</v>
+        <v>60</v>
+      </c>
+      <c r="F2" t="s" s="53">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s" s="59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s" s="65">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s" s="143">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="17" t="s">
+      <c r="D5" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s" s="62">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s" s="149">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="17" t="s">
+      <c r="E6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s" s="68">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B7" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" t="s" s="146">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s" s="152">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>56</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" t="s" s="155">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F7" t="s" s="71">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1496,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1506,78 +1429,78 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.796875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="24.46484375" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="7.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="44" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="135" t="s">
         <v>83</v>
       </c>
+      <c r="E2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="136" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1611,115 +1534,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="138" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="E3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="139" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="140" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="141" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="142" t="s">
-        <v>61</v>
+      <c r="F6" s="58" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1754,90 +1677,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="I1" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="40" t="s">
+      <c r="H2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" s="144" t="s">
-        <v>61</v>
+      <c r="I2" s="60" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="40" t="s">
+      <c r="D3" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="145" t="s">
-        <v>61</v>
+      <c r="I3" s="61" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1870,63 +1793,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="147" t="s">
-        <v>61</v>
+      <c r="F2" s="63" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="148" t="s">
-        <v>61</v>
+      <c r="D3" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="64" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1958,54 +1881,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="150" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="151" t="s">
-        <v>61</v>
+      <c r="D3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -2033,77 +1956,77 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
     <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
-    <col min="6" max="6" customWidth="true" style="37" width="69.53125"/>
+    <col min="6" max="6" customWidth="true" style="36" width="69.53125"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="6.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="153" t="s">
-        <v>61</v>
+      <c r="G2" s="69" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="B3" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="154" t="s">
-        <v>61</v>
+      <c r="D3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated exception handling in methods
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="88">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>33.33 %</t>
+  </si>
+  <si>
+    <t>0.0 %</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -582,6 +585,11 @@
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -749,7 +757,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -866,6 +874,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1290,10 +1308,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s" s="53">
-        <v>59</v>
+        <v>87</v>
+      </c>
+      <c r="F2" t="s" s="81">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1476,8 +1494,8 @@
       <c r="F2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="51" t="s">
-        <v>59</v>
+      <c r="G2" s="78" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1499,8 +1517,8 @@
       <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="52" t="s">
-        <v>59</v>
+      <c r="G3" s="80" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added driver factory & browser factory classes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="89">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t>0.0 %</t>
+  </si>
+  <si>
+    <t>66.67 %</t>
   </si>
 </sst>
 </file>
@@ -757,7 +760,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="382">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -889,6 +892,283 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1331,10 +1611,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s" s="86">
-        <v>81</v>
+        <v>60</v>
+      </c>
+      <c r="F2" t="s" s="363">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1353,7 +1633,7 @@
       <c r="E3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s" s="92">
+      <c r="F3" t="s" s="369">
         <v>59</v>
       </c>
     </row>
@@ -1373,7 +1653,7 @@
       <c r="E4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F4" t="s" s="98">
+      <c r="F4" t="s" s="375">
         <v>59</v>
       </c>
     </row>
@@ -1393,7 +1673,7 @@
       <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" t="s" s="95">
+      <c r="F5" t="s" s="372">
         <v>59</v>
       </c>
     </row>
@@ -1413,7 +1693,7 @@
       <c r="E6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F6" t="s" s="101">
+      <c r="F6" t="s" s="378">
         <v>59</v>
       </c>
     </row>
@@ -1433,7 +1713,7 @@
       <c r="E7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F7" t="s" s="104">
+      <c r="F7" t="s" s="381">
         <v>59</v>
       </c>
     </row>
@@ -1517,8 +1797,8 @@
       <c r="F2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="83" t="s">
-        <v>81</v>
+      <c r="G2" s="361" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1540,8 +1820,8 @@
       <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="85" t="s">
-        <v>81</v>
+      <c r="G3" s="362" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1890,7 @@
       <c r="E2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="364" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1630,7 +1910,7 @@
       <c r="E3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="365" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1646,7 +1926,7 @@
       <c r="E4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="89" t="s">
+      <c r="F4" s="366" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1664,7 +1944,7 @@
       <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="90" t="s">
+      <c r="F5" s="367" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1682,7 +1962,7 @@
       <c r="E6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="91" t="s">
+      <c r="F6" s="368" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1771,7 +2051,7 @@
       <c r="H2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="370" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1800,7 +2080,7 @@
       <c r="H3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="94" t="s">
+      <c r="I3" s="371" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1869,7 +2149,7 @@
       <c r="E2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="373" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1889,7 +2169,7 @@
       <c r="E3" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="374" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1951,7 +2231,7 @@
       <c r="D2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="376" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1968,7 +2248,7 @@
       <c r="D3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="100" t="s">
+      <c r="E3" s="377" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2043,7 +2323,7 @@
       <c r="F2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="102" t="s">
+      <c r="G2" s="379" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2066,7 +2346,7 @@
       <c r="F3" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="103" t="s">
+      <c r="G3" s="380" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed static web pages for sample website
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D670B551-72CD-4037-9CA8-05D33E6C6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811CC26E-CAEB-4C0D-8417-188F88745E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Play course overview</t>
   </si>
   <si>
-    <t xml:space="preserve">Java </t>
-  </si>
-  <si>
     <t>Custom</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>TC_0006_2</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>https://nirajt03.github.io/sample-website/</t>
   </si>
   <si>
@@ -412,13 +406,7 @@
     <t>pragyan@123</t>
   </si>
   <si>
-    <t>33.33 %</t>
-  </si>
-  <si>
-    <t>0.0 %</t>
-  </si>
-  <si>
-    <t>66.67 %</t>
+    <t xml:space="preserve">Java Fundamentals: The Java Language </t>
   </si>
 </sst>
 </file>
@@ -530,7 +518,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -583,16 +571,6 @@
         <fgColor indexed="50"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -760,7 +738,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="406">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -846,371 +824,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1509,8 +1125,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
@@ -1518,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1542,8 +1158,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.19921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -1558,8 +1174,8 @@
       <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>82</v>
+      <c r="B2" s="41" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1593,12 +1209,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.1328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1637,7 +1253,7 @@
       <c r="E2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s" s="387">
+      <c r="F2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1657,7 +1273,7 @@
       <c r="E3" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s" s="393">
+      <c r="F3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1677,7 +1293,7 @@
       <c r="E4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F4" t="s" s="399">
+      <c r="F4" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1697,7 +1313,7 @@
       <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" t="s" s="396">
+      <c r="F5" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1717,7 +1333,7 @@
       <c r="E6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F6" t="s" s="402">
+      <c r="F6" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1737,7 +1353,7 @@
       <c r="E7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F7" t="s" s="405">
+      <c r="F7" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1764,19 +1380,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.46484375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -1786,7 +1402,7 @@
       <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -1809,19 +1425,19 @@
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="43" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>85</v>
       </c>
       <c r="F2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="385" t="s">
+      <c r="G2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1830,21 +1446,21 @@
         <v>19</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="386" t="s">
+      <c r="G3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1870,12 +1486,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.06640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.265625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1914,7 +1530,7 @@
       <c r="E2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="388" t="s">
+      <c r="F2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1934,7 +1550,7 @@
       <c r="E3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="389" t="s">
+      <c r="F3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1950,7 +1566,7 @@
       <c r="E4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="390" t="s">
+      <c r="F4" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1968,7 +1584,7 @@
       <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="391" t="s">
+      <c r="F5" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1986,7 +1602,7 @@
       <c r="E6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="392" t="s">
+      <c r="F6" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2006,19 +1622,19 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
-    <col min="6" max="6" customWidth="true" width="69.46484375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.59765625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.46484375" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
@@ -2075,7 +1691,7 @@
       <c r="H2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="394" t="s">
+      <c r="I2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2084,7 +1700,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>23</v>
@@ -2104,7 +1720,7 @@
       <c r="H3" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="395" t="s">
+      <c r="I3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2129,12 +1745,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.06640625"/>
-    <col min="5" max="5" customWidth="true" width="59.59765625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.59765625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -2173,7 +1789,7 @@
       <c r="E2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="397" t="s">
+      <c r="F2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2182,7 +1798,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>23</v>
@@ -2193,7 +1809,7 @@
       <c r="E3" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="398" t="s">
+      <c r="F3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2213,16 +1829,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -2253,9 +1869,9 @@
         <v>22</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="400" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2264,15 +1880,15 @@
         <v>19</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="401" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2297,12 +1913,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
-    <col min="6" max="6" customWidth="true" style="36" width="69.53125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.53125" style="36" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -2347,7 +1963,7 @@
       <c r="F2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="403" t="s">
+      <c r="G2" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2356,7 +1972,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>23</v>
@@ -2370,7 +1986,7 @@
       <c r="F3" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="404" t="s">
+      <c r="G3" s="26" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated utility jar and required changes in classes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niraj Tiwari\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AF0D97-9846-4FBB-80C6-C0196E29476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32B5FD-F539-4CB4-94D7-DC572BF42F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="95">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -496,7 +496,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,11 +560,6 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -732,7 +727,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,6 +816,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -843,73 +842,99 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1286,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,7 +1320,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="8.109375" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="33.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.21875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="7.21875" collapsed="true"/>
   </cols>
@@ -1336,7 +1361,7 @@
       <c r="E2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s" s="110">
+      <c r="F2" t="s" s="138">
         <v>83</v>
       </c>
     </row>
@@ -1356,7 +1381,7 @@
       <c r="E3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s" s="116">
+      <c r="F3" t="s" s="144">
         <v>83</v>
       </c>
     </row>
@@ -1376,7 +1401,7 @@
       <c r="E4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="s" s="122">
+      <c r="F4" t="s" s="150">
         <v>83</v>
       </c>
     </row>
@@ -1396,7 +1421,7 @@
       <c r="E5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F5" t="s" s="119">
+      <c r="F5" t="s" s="147">
         <v>83</v>
       </c>
     </row>
@@ -1416,12 +1441,12 @@
       <c r="E6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F6" t="s" s="125">
+      <c r="F6" t="s" s="153">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="66" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -1434,10 +1459,10 @@
         <v>47</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" t="s" s="128">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="F7" t="s" s="156">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1489,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,7 +1552,7 @@
       <c r="G2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="136" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1553,7 +1578,7 @@
       <c r="G3" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="109" t="s">
+      <c r="H3" s="137" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1574,7 +1599,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+      <selection activeCell="F1" sqref="F1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,13 +1649,13 @@
       <c r="D2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="43" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="111" t="s">
+      <c r="G2" s="139" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1647,13 +1672,13 @@
       <c r="D3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="64" t="s">
+      <c r="E3" s="43" t="s">
         <v>37</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="112" t="s">
+      <c r="G3" s="140" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1666,13 +1691,13 @@
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="43" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="113" t="s">
+      <c r="G4" s="141" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1687,13 +1712,13 @@
         <v>22</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="43" t="s">
         <v>37</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="114" t="s">
+      <c r="G5" s="142" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1708,13 +1733,13 @@
       <c r="D6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="43" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="115" t="s">
+      <c r="G6" s="143" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1733,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,7 +1835,7 @@
       <c r="I2" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="117" t="s">
+      <c r="J2" s="145" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1842,7 +1867,7 @@
       <c r="I3" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="118" t="s">
+      <c r="J3" s="146" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1862,7 +1887,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,7 +1942,7 @@
       <c r="F2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="120" t="s">
+      <c r="G2" s="148" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1940,7 +1965,7 @@
       <c r="F3" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="121" t="s">
+      <c r="G3" s="149" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1961,7 +1986,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E1" sqref="E1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2009,7 +2034,7 @@
       <c r="E2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="151" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2029,7 +2054,7 @@
       <c r="E3" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="152" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2048,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2108,10 +2133,10 @@
       <c r="F2" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="126" t="s">
+      <c r="H2" s="154" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2134,10 +2159,10 @@
       <c r="F3" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="127" t="s">
+      <c r="H3" s="155" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made base classes abstract
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="96">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>TCs-016,TCs-017,TCs-018,TCs-019,TCs-020</t>
+  </si>
+  <si>
+    <t>0.0 %</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +563,11 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -727,7 +735,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -956,6 +964,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
@@ -1403,7 +1435,7 @@
       <c r="E2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s" s="180">
+      <c r="F2" t="s" s="219">
         <v>83</v>
       </c>
     </row>
@@ -1443,7 +1475,7 @@
       <c r="E4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="s" s="192">
+      <c r="F4" t="s" s="222">
         <v>83</v>
       </c>
     </row>
@@ -1594,7 +1626,7 @@
       <c r="G2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="217" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1620,7 +1652,7 @@
       <c r="G3" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="179" t="s">
+      <c r="H3" s="218" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1984,7 +2016,7 @@
       <c r="F2" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="190" t="s">
+      <c r="G2" s="220" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2007,7 +2039,7 @@
       <c r="F3" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="191" t="s">
+      <c r="G3" s="221" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>